<commit_message>
bookeeping works! Test Graphs?
</commit_message>
<xml_diff>
--- a/summaries/run_report.xlsx
+++ b/summaries/run_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X31"/>
+  <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,6 +554,11 @@
           <t>show_res</t>
         </is>
       </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>from_scratch</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="b">
@@ -652,6 +657,7 @@
       </c>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="b">
@@ -750,6 +756,7 @@
       </c>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="b">
@@ -848,6 +855,7 @@
       </c>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="b">
@@ -946,6 +954,7 @@
       </c>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="b">
@@ -1044,6 +1053,7 @@
       </c>
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="b">
@@ -1142,6 +1152,7 @@
       </c>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="b">
@@ -1240,6 +1251,7 @@
       </c>
       <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="b">
@@ -1338,6 +1350,7 @@
       </c>
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="b">
@@ -1436,6 +1449,7 @@
       </c>
       <c r="W10" t="inlineStr"/>
       <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="b">
@@ -1534,6 +1548,7 @@
       </c>
       <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="b">
@@ -1632,6 +1647,7 @@
       </c>
       <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="b">
@@ -1730,6 +1746,7 @@
       </c>
       <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="b">
@@ -1832,6 +1849,7 @@
         </is>
       </c>
       <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="b">
@@ -1934,6 +1952,7 @@
         </is>
       </c>
       <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="b">
@@ -2036,6 +2055,7 @@
         </is>
       </c>
       <c r="X16" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="b">
@@ -2138,6 +2158,7 @@
         </is>
       </c>
       <c r="X17" t="inlineStr"/>
+      <c r="Y17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="b">
@@ -2240,6 +2261,7 @@
         </is>
       </c>
       <c r="X18" t="inlineStr"/>
+      <c r="Y18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="b">
@@ -2342,6 +2364,7 @@
         </is>
       </c>
       <c r="X19" t="inlineStr"/>
+      <c r="Y19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="b">
@@ -2444,6 +2467,7 @@
         </is>
       </c>
       <c r="X20" t="inlineStr"/>
+      <c r="Y20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="b">
@@ -2546,6 +2570,7 @@
         </is>
       </c>
       <c r="X21" t="inlineStr"/>
+      <c r="Y21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="b">
@@ -2648,6 +2673,7 @@
         </is>
       </c>
       <c r="X22" t="inlineStr"/>
+      <c r="Y22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="b">
@@ -2750,6 +2776,7 @@
         </is>
       </c>
       <c r="X23" t="inlineStr"/>
+      <c r="Y23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="b">
@@ -2852,6 +2879,7 @@
         </is>
       </c>
       <c r="X24" t="inlineStr"/>
+      <c r="Y24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="b">
@@ -2954,6 +2982,7 @@
         </is>
       </c>
       <c r="X25" t="inlineStr"/>
+      <c r="Y25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="b">
@@ -3056,6 +3085,7 @@
         </is>
       </c>
       <c r="X26" t="inlineStr"/>
+      <c r="Y26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="b">
@@ -3158,6 +3188,7 @@
         </is>
       </c>
       <c r="X27" t="inlineStr"/>
+      <c r="Y27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="b">
@@ -3260,6 +3291,7 @@
         </is>
       </c>
       <c r="X28" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="b">
@@ -3362,6 +3394,7 @@
         </is>
       </c>
       <c r="X29" t="inlineStr"/>
+      <c r="Y29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="b">
@@ -3464,6 +3497,7 @@
         </is>
       </c>
       <c r="X30" t="inlineStr"/>
+      <c r="Y30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="b">
@@ -3565,8 +3599,324 @@
           <t>xavier</t>
         </is>
       </c>
-      <c r="X31" t="b">
+      <c r="X31" t="n">
         <v>1</v>
+      </c>
+      <c r="Y31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="b">
+        <v>0</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>500</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G32" t="n">
+        <v>3</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>mlp_lin</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S32" t="n">
+        <v>10</v>
+      </c>
+      <c r="T32" t="n">
+        <v>3000</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="V32" t="inlineStr">
+        <is>
+          <t>run_031</t>
+        </is>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>xavier</t>
+        </is>
+      </c>
+      <c r="X32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="b">
+        <v>0</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>500</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G33" t="n">
+        <v>3</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>mlp_lin</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S33" t="n">
+        <v>10</v>
+      </c>
+      <c r="T33" t="n">
+        <v>3000</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="V33" t="inlineStr">
+        <is>
+          <t>run_032</t>
+        </is>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>xavier</t>
+        </is>
+      </c>
+      <c r="X33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="b">
+        <v>0</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>500</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G34" t="n">
+        <v>3</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>mlp_lin</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S34" t="n">
+        <v>200</v>
+      </c>
+      <c r="T34" t="n">
+        <v>3000</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="V34" t="inlineStr">
+        <is>
+          <t>run_033</t>
+        </is>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>xavier</t>
+        </is>
+      </c>
+      <c r="X34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ready for last 2 weeks push!! Readme PLAN!
</commit_message>
<xml_diff>
--- a/summaries/run_report.xlsx
+++ b/summaries/run_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:AA48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -559,6 +559,16 @@
           <t>from_scratch</t>
         </is>
       </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>seed</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="b">
@@ -658,6 +668,8 @@
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="b">
@@ -757,6 +769,8 @@
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
       <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="b">
@@ -856,6 +870,8 @@
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="b">
@@ -955,6 +971,8 @@
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="b">
@@ -1054,6 +1072,8 @@
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
       <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="b">
@@ -1153,6 +1173,8 @@
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="b">
@@ -1252,6 +1274,8 @@
       <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr"/>
       <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="b">
@@ -1351,6 +1375,8 @@
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="b">
@@ -1450,6 +1476,8 @@
       <c r="W10" t="inlineStr"/>
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="b">
@@ -1549,6 +1577,8 @@
       <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="b">
@@ -1648,6 +1678,8 @@
       <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr"/>
       <c r="Y12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="b">
@@ -1747,6 +1779,8 @@
       <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
       <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="b">
@@ -1850,6 +1884,8 @@
       </c>
       <c r="X14" t="inlineStr"/>
       <c r="Y14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="b">
@@ -1953,6 +1989,8 @@
       </c>
       <c r="X15" t="inlineStr"/>
       <c r="Y15" t="inlineStr"/>
+      <c r="Z15" t="inlineStr"/>
+      <c r="AA15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="b">
@@ -2056,6 +2094,8 @@
       </c>
       <c r="X16" t="inlineStr"/>
       <c r="Y16" t="inlineStr"/>
+      <c r="Z16" t="inlineStr"/>
+      <c r="AA16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="b">
@@ -2159,6 +2199,8 @@
       </c>
       <c r="X17" t="inlineStr"/>
       <c r="Y17" t="inlineStr"/>
+      <c r="Z17" t="inlineStr"/>
+      <c r="AA17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="b">
@@ -2262,6 +2304,8 @@
       </c>
       <c r="X18" t="inlineStr"/>
       <c r="Y18" t="inlineStr"/>
+      <c r="Z18" t="inlineStr"/>
+      <c r="AA18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="b">
@@ -2365,6 +2409,8 @@
       </c>
       <c r="X19" t="inlineStr"/>
       <c r="Y19" t="inlineStr"/>
+      <c r="Z19" t="inlineStr"/>
+      <c r="AA19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="b">
@@ -2468,6 +2514,8 @@
       </c>
       <c r="X20" t="inlineStr"/>
       <c r="Y20" t="inlineStr"/>
+      <c r="Z20" t="inlineStr"/>
+      <c r="AA20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="b">
@@ -2571,6 +2619,8 @@
       </c>
       <c r="X21" t="inlineStr"/>
       <c r="Y21" t="inlineStr"/>
+      <c r="Z21" t="inlineStr"/>
+      <c r="AA21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="b">
@@ -2674,6 +2724,8 @@
       </c>
       <c r="X22" t="inlineStr"/>
       <c r="Y22" t="inlineStr"/>
+      <c r="Z22" t="inlineStr"/>
+      <c r="AA22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="b">
@@ -2777,6 +2829,8 @@
       </c>
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr"/>
+      <c r="Z23" t="inlineStr"/>
+      <c r="AA23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="b">
@@ -2880,6 +2934,8 @@
       </c>
       <c r="X24" t="inlineStr"/>
       <c r="Y24" t="inlineStr"/>
+      <c r="Z24" t="inlineStr"/>
+      <c r="AA24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="b">
@@ -2983,6 +3039,8 @@
       </c>
       <c r="X25" t="inlineStr"/>
       <c r="Y25" t="inlineStr"/>
+      <c r="Z25" t="inlineStr"/>
+      <c r="AA25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="b">
@@ -3086,6 +3144,8 @@
       </c>
       <c r="X26" t="inlineStr"/>
       <c r="Y26" t="inlineStr"/>
+      <c r="Z26" t="inlineStr"/>
+      <c r="AA26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="b">
@@ -3189,6 +3249,8 @@
       </c>
       <c r="X27" t="inlineStr"/>
       <c r="Y27" t="inlineStr"/>
+      <c r="Z27" t="inlineStr"/>
+      <c r="AA27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="b">
@@ -3292,6 +3354,8 @@
       </c>
       <c r="X28" t="inlineStr"/>
       <c r="Y28" t="inlineStr"/>
+      <c r="Z28" t="inlineStr"/>
+      <c r="AA28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="b">
@@ -3395,6 +3459,8 @@
       </c>
       <c r="X29" t="inlineStr"/>
       <c r="Y29" t="inlineStr"/>
+      <c r="Z29" t="inlineStr"/>
+      <c r="AA29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="b">
@@ -3498,6 +3564,8 @@
       </c>
       <c r="X30" t="inlineStr"/>
       <c r="Y30" t="inlineStr"/>
+      <c r="Z30" t="inlineStr"/>
+      <c r="AA30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="b">
@@ -3603,6 +3671,8 @@
         <v>1</v>
       </c>
       <c r="Y31" t="inlineStr"/>
+      <c r="Z31" t="inlineStr"/>
+      <c r="AA31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="b">
@@ -3708,6 +3778,8 @@
       <c r="Y32" t="n">
         <v>1</v>
       </c>
+      <c r="Z32" t="inlineStr"/>
+      <c r="AA32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="b">
@@ -3813,6 +3885,8 @@
       <c r="Y33" t="n">
         <v>0</v>
       </c>
+      <c r="Z33" t="inlineStr"/>
+      <c r="AA33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="b">
@@ -3917,6 +3991,1532 @@
       </c>
       <c r="Y34" t="n">
         <v>0</v>
+      </c>
+      <c r="Z34" t="inlineStr"/>
+      <c r="AA34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="b">
+        <v>0</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>500</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G35" t="n">
+        <v>3</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>mlp_lin</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S35" t="n">
+        <v>200</v>
+      </c>
+      <c r="T35" t="n">
+        <v>3000</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="V35" t="inlineStr">
+        <is>
+          <t>run_034</t>
+        </is>
+      </c>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>xavier</t>
+        </is>
+      </c>
+      <c r="X35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z35" t="inlineStr"/>
+      <c r="AA35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="b">
+        <v>0</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>500</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G36" t="n">
+        <v>3</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>mlp_lin</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S36" t="n">
+        <v>200</v>
+      </c>
+      <c r="T36" t="n">
+        <v>3000</v>
+      </c>
+      <c r="U36" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="V36" t="inlineStr">
+        <is>
+          <t>run_035</t>
+        </is>
+      </c>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>xavier</t>
+        </is>
+      </c>
+      <c r="X36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z36" t="inlineStr"/>
+      <c r="AA36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>500</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G37" t="n">
+        <v>3</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>deep_mlp</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>[10, 1]</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S37" t="n">
+        <v>200</v>
+      </c>
+      <c r="T37" t="n">
+        <v>3000</v>
+      </c>
+      <c r="U37" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="V37" t="inlineStr">
+        <is>
+          <t>run_036</t>
+        </is>
+      </c>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>xavier</t>
+        </is>
+      </c>
+      <c r="X37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z37" t="inlineStr"/>
+      <c r="AA37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="b">
+        <v>0</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>500</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G38" t="n">
+        <v>3</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>deep_mlp</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>[10, 1]</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S38" t="n">
+        <v>200</v>
+      </c>
+      <c r="T38" t="n">
+        <v>3000</v>
+      </c>
+      <c r="U38" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="V38" t="inlineStr">
+        <is>
+          <t>run_037</t>
+        </is>
+      </c>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>xavier</t>
+        </is>
+      </c>
+      <c r="X38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z38" t="inlineStr"/>
+      <c r="AA38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="b">
+        <v>0</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>500</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G39" t="n">
+        <v>3</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>deep_mlp</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>[10, 1]</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S39" t="n">
+        <v>200</v>
+      </c>
+      <c r="T39" t="n">
+        <v>600</v>
+      </c>
+      <c r="U39" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="V39" t="inlineStr">
+        <is>
+          <t>run_038</t>
+        </is>
+      </c>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>xavier</t>
+        </is>
+      </c>
+      <c r="X39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z39" t="inlineStr"/>
+      <c r="AA39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="b">
+        <v>0</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>500</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G40" t="n">
+        <v>3</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>deep_mlp</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S40" t="n">
+        <v>200</v>
+      </c>
+      <c r="T40" t="n">
+        <v>600</v>
+      </c>
+      <c r="U40" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="V40" t="inlineStr">
+        <is>
+          <t>run_039</t>
+        </is>
+      </c>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>xavier</t>
+        </is>
+      </c>
+      <c r="X40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y40" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z40" t="n">
+        <v>42</v>
+      </c>
+      <c r="AA40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>500</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G41" t="n">
+        <v>3</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S41" t="n">
+        <v>200</v>
+      </c>
+      <c r="T41" t="n">
+        <v>1000</v>
+      </c>
+      <c r="U41" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="V41" t="inlineStr">
+        <is>
+          <t>run_040</t>
+        </is>
+      </c>
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="X41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y41" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z41" t="n">
+        <v>42</v>
+      </c>
+      <c r="AA41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="b">
+        <v>0</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>500</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G42" t="n">
+        <v>3</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>mlp_big_batch</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S42" t="n">
+        <v>1</v>
+      </c>
+      <c r="T42" t="n">
+        <v>4500</v>
+      </c>
+      <c r="U42" t="n">
+        <v>0.0002</v>
+      </c>
+      <c r="V42" t="inlineStr">
+        <is>
+          <t>run_041</t>
+        </is>
+      </c>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>xavier</t>
+        </is>
+      </c>
+      <c r="X42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z42" t="n">
+        <v>42</v>
+      </c>
+      <c r="AA42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="b">
+        <v>0</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>500</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G43" t="n">
+        <v>3</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>mlp_big_batch</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S43" t="n">
+        <v>100</v>
+      </c>
+      <c r="T43" t="n">
+        <v>4500</v>
+      </c>
+      <c r="U43" t="n">
+        <v>0.0002</v>
+      </c>
+      <c r="V43" t="inlineStr">
+        <is>
+          <t>run_042</t>
+        </is>
+      </c>
+      <c r="W43" t="inlineStr">
+        <is>
+          <t>xavier</t>
+        </is>
+      </c>
+      <c r="X43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z43" t="n">
+        <v>42</v>
+      </c>
+      <c r="AA43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="b">
+        <v>0</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>500</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G44" t="n">
+        <v>3</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>mlp_big_batch</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>tanh</t>
+        </is>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S44" t="n">
+        <v>200</v>
+      </c>
+      <c r="T44" t="n">
+        <v>4500</v>
+      </c>
+      <c r="U44" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="V44" t="inlineStr">
+        <is>
+          <t>run_043</t>
+        </is>
+      </c>
+      <c r="W44" t="inlineStr">
+        <is>
+          <t>xavier</t>
+        </is>
+      </c>
+      <c r="X44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y44" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z44" t="n">
+        <v>42</v>
+      </c>
+      <c r="AA44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="b">
+        <v>0</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>500</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G45" t="n">
+        <v>3</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>mlp_relu_tan</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>relu</t>
+        </is>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S45" t="n">
+        <v>200</v>
+      </c>
+      <c r="T45" t="n">
+        <v>4500</v>
+      </c>
+      <c r="U45" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="V45" t="inlineStr">
+        <is>
+          <t>run_044</t>
+        </is>
+      </c>
+      <c r="W45" t="inlineStr">
+        <is>
+          <t>xavier</t>
+        </is>
+      </c>
+      <c r="X45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y45" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z45" t="n">
+        <v>42</v>
+      </c>
+      <c r="AA45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="b">
+        <v>0</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>500</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G46" t="n">
+        <v>3</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>mlp_comparison</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>relu</t>
+        </is>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S46" t="n">
+        <v>250</v>
+      </c>
+      <c r="T46" t="n">
+        <v>4500</v>
+      </c>
+      <c r="U46" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="V46" t="inlineStr">
+        <is>
+          <t>run_045</t>
+        </is>
+      </c>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t>xavier</t>
+        </is>
+      </c>
+      <c r="X46" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y46" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z46" t="n">
+        <v>42</v>
+      </c>
+      <c r="AA46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="b">
+        <v>0</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>500</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G47" t="n">
+        <v>3</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>mlp_comparison</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>relu</t>
+        </is>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S47" t="n">
+        <v>250</v>
+      </c>
+      <c r="T47" t="n">
+        <v>600</v>
+      </c>
+      <c r="U47" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="V47" t="inlineStr">
+        <is>
+          <t>run_046</t>
+        </is>
+      </c>
+      <c r="W47" t="inlineStr">
+        <is>
+          <t>xavier</t>
+        </is>
+      </c>
+      <c r="X47" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y47" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z47" t="n">
+        <v>42</v>
+      </c>
+      <c r="AA47" t="inlineStr">
+        <is>
+          <t>sgd</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="b">
+        <v>0</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>runs_report.xlsx</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>['050']</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>500</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G48" t="n">
+        <v>3</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>mlp_comparison</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>fixed-grid</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>rk4</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>relu</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>[1, 3, 1]</t>
+        </is>
+      </c>
+      <c r="S48" t="n">
+        <v>1050</v>
+      </c>
+      <c r="T48" t="n">
+        <v>600</v>
+      </c>
+      <c r="U48" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="V48" t="inlineStr">
+        <is>
+          <t>run_047</t>
+        </is>
+      </c>
+      <c r="W48" t="inlineStr">
+        <is>
+          <t>xavier</t>
+        </is>
+      </c>
+      <c r="X48" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z48" t="n">
+        <v>42</v>
+      </c>
+      <c r="AA48" t="inlineStr">
+        <is>
+          <t>sgd</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>